<commit_message>
# 1.1 new look and feel #		Work in 7.3 and upper (temporary file is loaded in a different place) #		Compatible 7.5 (encode URL)
</commit_message>
<xml_diff>
--- a/tests/cover test V2.xlsx
+++ b/tests/cover test V2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\git\bonita-community\page_snowmobile\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="6135" windowHeight="2340"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -273,8 +278,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +376,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,7 +430,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,9 +462,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -483,6 +514,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -658,14 +707,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -675,7 +724,7 @@
     <col min="6" max="6" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -683,7 +732,7 @@
       <c r="D1" s="8"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:7" s="9" customFormat="1">
+    <row r="2" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -700,7 +749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -717,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -734,7 +783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -751,7 +800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -768,7 +817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -788,7 +837,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -808,7 +857,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -825,7 +874,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -842,7 +891,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -859,7 +908,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -876,7 +925,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -893,7 +942,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>13</v>
       </c>
@@ -910,7 +959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -930,7 +979,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1">
+    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
@@ -938,7 +987,7 @@
       <c r="D16" s="8"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f>A15+1</f>
         <v>15</v>
@@ -956,7 +1005,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f>A17+1</f>
         <v>16</v>
@@ -974,7 +1023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" ref="A19:A24" si="0">A18+1</f>
         <v>17</v>
@@ -992,7 +1041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1013,7 +1062,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1034,7 +1083,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1055,7 +1104,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1073,7 +1122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1091,7 +1140,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1">
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1148,7 @@
       <c r="D25" s="8"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f>A24+1</f>
         <v>23</v>
@@ -1120,7 +1169,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f>A26+1</f>
         <v>24</v>
@@ -1138,7 +1187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" ref="A28:A29" si="1">A27+1</f>
         <v>25</v>
@@ -1159,7 +1208,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1180,7 +1229,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1237,7 @@
       <c r="D30" s="8"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f>A29+1</f>
         <v>27</v>
@@ -1206,7 +1255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f>A31+1</f>
         <v>28</v>
@@ -1224,7 +1273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="7" customFormat="1">
+    <row r="33" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>70</v>
       </c>
@@ -1232,7 +1281,7 @@
       <c r="D33" s="8"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f>A32+1</f>
         <v>29</v>
@@ -1250,7 +1299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f>A34+1</f>
         <v>30</v>
@@ -1269,7 +1318,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" ref="A36:A38" si="2">A35+1</f>
         <v>31</v>
@@ -1284,7 +1333,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1299,7 +1348,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1327,24 +1376,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>